<commit_message>
Update order of height steps.
Leave out the partial one.
</commit_message>
<xml_diff>
--- a/MosaicReconstruction/example/param_files/tissue58.xlsx
+++ b/MosaicReconstruction/example/param_files/tissue58.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -91,16 +91,16 @@
     <t xml:space="preserve">z3_x3</t>
   </si>
   <si>
-    <t xml:space="preserve">y4_x0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y4_x1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y4_x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y4_x3</t>
+    <t xml:space="preserve">z4_x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z4_x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z4_x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z4_x3</t>
   </si>
   <si>
     <t xml:space="preserve">z5_x0</t>
@@ -122,12 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">z6_x1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z6_x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z6_x3</t>
   </si>
 </sst>
 </file>
@@ -137,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -159,12 +153,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,13 +197,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -246,10 +230,10 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="79.45"/>
@@ -289,7 +273,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -306,7 +290,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -323,7 +307,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -340,7 +324,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -356,10 +340,10 @@
       <c r="B6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -373,10 +357,10 @@
       <c r="B7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -390,10 +374,10 @@
       <c r="B8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -407,10 +391,10 @@
       <c r="B9" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="0" t="n">
@@ -424,10 +408,10 @@
       <c r="B10" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="0" t="n">
@@ -441,10 +425,10 @@
       <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="0" t="n">
@@ -458,10 +442,10 @@
       <c r="B12" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="0" t="n">
@@ -475,10 +459,10 @@
       <c r="B13" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="0" t="n">
@@ -492,10 +476,10 @@
       <c r="B14" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="0" t="n">
@@ -509,10 +493,10 @@
       <c r="B15" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="0" t="n">
@@ -526,10 +510,10 @@
       <c r="B16" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="0" t="n">
@@ -543,10 +527,10 @@
       <c r="B17" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="0" t="n">
@@ -560,10 +544,10 @@
       <c r="B18" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="0" t="n">
@@ -577,10 +561,10 @@
       <c r="B19" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="0" t="n">
@@ -594,10 +578,10 @@
       <c r="B20" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="0" t="n">
@@ -611,10 +595,10 @@
       <c r="B21" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="0" t="n">
@@ -628,10 +612,10 @@
       <c r="B22" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="0" t="n">
@@ -645,10 +629,10 @@
       <c r="B23" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="0" t="n">
@@ -662,10 +646,10 @@
       <c r="B24" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="0" t="n">
@@ -679,10 +663,10 @@
       <c r="B25" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="0" t="n">
@@ -696,10 +680,10 @@
       <c r="B26" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E26" s="0" t="n">
@@ -713,10 +697,10 @@
       <c r="B27" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="0" t="n">
@@ -724,134 +708,108 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>3</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>4</v>
-      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E46" s="3"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E47" s="3"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E48" s="3"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="3"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="3"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E51" s="3"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="3"/>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="3"/>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="3"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="3"/>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E56" s="3"/>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E57" s="3"/>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="3"/>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E59" s="3"/>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E60" s="3"/>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E61" s="3"/>
+      <c r="E61" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update info file for tissue58.
</commit_message>
<xml_diff>
--- a/MosaicReconstruction/example/param_files/tissue58.xlsx
+++ b/MosaicReconstruction/example/param_files/tissue58.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t xml:space="preserve">z6_x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z6_x2_dummy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z6_x3_dummy</t>
   </si>
 </sst>
 </file>
@@ -230,15 +236,15 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="79.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
@@ -708,12 +714,38 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C34" s="2"/>

</xml_diff>

<commit_message>
Fix error in tissue58 xlsx.
</commit_message>
<xml_diff>
--- a/MosaicReconstruction/example/param_files/tissue58.xlsx
+++ b/MosaicReconstruction/example/param_files/tissue58.xlsx
@@ -124,10 +124,10 @@
     <t xml:space="preserve">z6_x1</t>
   </si>
   <si>
-    <t xml:space="preserve">z6_x2_dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z6_x3_dummy</t>
+    <t xml:space="preserve">z6_x0002__x2_dummy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z6_x0003__x3_dummy</t>
   </si>
 </sst>
 </file>
@@ -236,15 +236,15 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="79.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>

</xml_diff>